<commit_message>
Adds extra sheet in Excel file for prescribed fertilizer application
</commit_message>
<xml_diff>
--- a/APU_5_2017_soybeans_clip (1).xlsx
+++ b/APU_5_2017_soybeans_clip (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ddrive\atkins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markd.LAPTOP-UMFS8BI9\PycharmProjects\USDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11F2D21E-1014-46E7-BFE5-BEA6925A2F5A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AD9D1B-4F06-403C-AEFC-0B9B7D526B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7545" yWindow="3975" windowWidth="17280" windowHeight="9060"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APU_5_2017_soybeans_clip" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -568,7 +568,15 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -877,10 +885,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CI35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="CC37" sqref="CC37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -8560,6 +8570,12 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A7:CI35">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
+      <formula>154.46</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>